<commit_message>
Add filter and get name  to get Scania popSize
</commit_message>
<xml_diff>
--- a/docs/PlagueProject/data/allParishesScania.xlsx
+++ b/docs/PlagueProject/data/allParishesScania.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/polislizarralde/PythonPlayground/docs/PlagueProject/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/polislizarralde/PythonMathematicalModeling/docs/PlagueProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0940BE5-10D6-9B45-ABA5-4492EBB295E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C32B5-9E6C-134D-84A7-F351A1F67F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="23620" windowWidth="27640" windowHeight="16940" xr2:uid="{3AB66EBA-79BB-D144-A3DB-F3ED8F1BA0A2}"/>
+    <workbookView xWindow="4080" yWindow="22660" windowWidth="27640" windowHeight="16940" xr2:uid="{3AB66EBA-79BB-D144-A3DB-F3ED8F1BA0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>Vallby</t>
   </si>
   <si>
-    <t>Östra Nöbbelov</t>
-  </si>
-  <si>
     <t>Östra Tommarp</t>
   </si>
   <si>
@@ -1314,6 +1311,9 @@
   </si>
   <si>
     <t>Österslöv</t>
+  </si>
+  <si>
+    <t>Östra Nöbbelöv</t>
   </si>
 </sst>
 </file>
@@ -1712,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3A5E15-205D-8D42-B605-CC95721B2F67}">
   <dimension ref="A1:C399"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2292,7 +2292,7 @@
         <v>49</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>58</v>
+        <v>425</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2303,7 +2303,7 @@
         <v>49</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2314,7 +2314,7 @@
         <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2322,10 +2322,10 @@
         <v>3</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2333,10 +2333,10 @@
         <v>3</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2344,10 +2344,10 @@
         <v>3</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2355,10 +2355,10 @@
         <v>3</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2366,10 +2366,10 @@
         <v>3</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2377,10 +2377,10 @@
         <v>3</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2388,3728 +2388,3728 @@
         <v>3</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C62" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C64" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C65" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C66" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C67" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C68" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C69" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C70" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C71" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C72" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C73" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C74" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C75" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C77" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C78" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C79" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C121" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B145" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B197" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B197" s="3" t="s">
+      <c r="C197" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B198" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B198" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C198" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B199" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B199" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C199" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B200" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B200" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C200" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B201" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B201" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C201" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B202" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B202" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C202" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B203" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B203" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C203" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B204" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B204" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C204" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B205" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C205" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A206" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B206" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B206" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C206" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B207" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C207" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B208" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B208" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C208" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B209" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B209" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C209" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B210" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B210" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C210" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B211" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B211" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C211" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B212" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C212" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B213" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B213" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C213" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B214" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B214" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C214" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B215" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B215" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C215" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B216" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B216" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C216" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B217" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B217" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C217" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B218" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B218" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="C218" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B219" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C219" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A226" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B238" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B238" s="3" t="s">
+      <c r="C238" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="C238" s="6" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B239" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B239" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C239" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B240" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B240" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C240" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B241" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B241" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C241" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B242" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C242" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B243" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C243" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B244" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B244" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C244" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B245" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B245" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C245" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B246" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="C246" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B247" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C247" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="C247" s="6" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C248" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C251" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C252" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B272" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C272" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="C272" s="3" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C286" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B288" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C288" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="C288" s="3" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C289" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C294" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A300" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C300" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B305" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C305" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="C305" s="3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C306" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C307" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C308" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C309" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C310" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C311" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C315" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C316" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C317" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C318" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B319" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C319" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="C319" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C320" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C321" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C322" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C323" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C324" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C327" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B328" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B328" s="3" t="s">
+      <c r="C328" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="C328" s="3" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B329" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B329" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C329" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B330" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B330" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C330" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B331" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B331" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C331" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B332" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B332" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C332" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B333" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B333" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C333" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B334" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B334" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C334" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B335" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B335" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C335" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B336" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B336" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C336" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B337" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B337" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C337" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B338" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B338" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C338" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B339" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B339" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C339" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B340" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B340" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C340" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B341" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B341" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C341" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B342" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B342" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C342" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B343" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B343" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C343" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B344" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C344" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B345" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B345" s="3" t="s">
-        <v>350</v>
-      </c>
       <c r="C345" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B346" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C346" s="3" t="s">
         <v>369</v>
-      </c>
-      <c r="C346" s="3" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C347" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C348" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C349" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C352" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C353" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C354" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C355" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C356" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C357" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C358" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C360" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C361" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C362" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C363" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C364" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C365" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C366" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C367" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A368" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C368" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B369" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C369" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="C369" s="3" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C372" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C373" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C374" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C375" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C376" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C377" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C378" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C379" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C380" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C381" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B382" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C382" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="C382" s="3" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C383" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C384" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C385" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C386" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C387" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A388" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C388" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C389" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C390" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A392" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C392" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A393" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C393" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C394" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C395" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C397" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C398" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C399" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change SkåneRegion for Region
</commit_message>
<xml_diff>
--- a/docs/PlagueProject/data/allParishesScania.xlsx
+++ b/docs/PlagueProject/data/allParishesScania.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/polislizarralde/PythonMathematicalModeling/docs/PlagueProject/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianapli/Desktop/PythonMathematicalModeling/docs/PlagueProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8520ADB-80EC-D648-BD90-C5E16025D43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A4348-C6C5-5B4B-9D55-422E60771DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="22100" windowWidth="28800" windowHeight="17500" xr2:uid="{3AB66EBA-79BB-D144-A3DB-F3ED8F1BA0A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{3AB66EBA-79BB-D144-A3DB-F3ED8F1BA0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1313,10 +1312,10 @@
     <t>ParishName</t>
   </si>
   <si>
-    <t>SkåneRegion</t>
-  </si>
-  <si>
     <t>Helsingborg</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -1715,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3A5E15-205D-8D42-B605-CC95721B2F67}">
   <dimension ref="A1:C399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A390" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1727,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4550,7 +4549,7 @@
         <v>260</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>